<commit_message>
Added an F&O Evaluator. It will create new stock files if it doesn't exist yet. Old one remains unchanged
</commit_message>
<xml_diff>
--- a/Stocks/3MINDIA.xlsx
+++ b/Stocks/3MINDIA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="35">
   <si>
     <t>Scrip</t>
   </si>
@@ -597,11 +597,10 @@
         <v>11362</v>
       </c>
       <c r="G2">
-        <f>_xll.TA_TYPPRICE(D2,E2,F2)</f>
         <v>11437.333333333334</v>
       </c>
       <c r="H2" t="e">
-        <f t="array" ref="H2:H82">_xll.TA_EMA(G2:G82,3)</f>
+        <f t="array" ref="H2:H104">_xll.TA_EMA(G2:G104,3)</f>
         <v>#N/A</v>
       </c>
       <c r="I2" t="e">
@@ -609,11 +608,11 @@
         <v>#N/A</v>
       </c>
       <c r="J2" t="e">
-        <f t="array" ref="J2:J82">_xll.TA_EMA(D2:D82,8)</f>
+        <f t="array" ref="J2:J104">_xll.TA_EMA(D2:D104,8)</f>
         <v>#N/A</v>
       </c>
       <c r="K2" t="e">
-        <f t="array" ref="K2:K82">_xll.TA_EMA(E2:E82,8)</f>
+        <f t="array" ref="K2:K104">_xll.TA_EMA(E2:E104,8)</f>
         <v>#N/A</v>
       </c>
       <c r="L2" t="e">
@@ -625,7 +624,7 @@
         <v>#N/A</v>
       </c>
       <c r="N2" t="e">
-        <f t="array" ref="N2:N82">_xll.TA_RSI(F2:F82,5)</f>
+        <f t="array" ref="N2:N104">_xll.TA_RSI(F2:F104,5)</f>
         <v>#N/A</v>
       </c>
       <c r="O2" t="e">
@@ -657,11 +656,11 @@
         <v>#N/A</v>
       </c>
       <c r="V2" t="e">
-        <f t="array" ref="V2:V82">_xll.TA_EMA(F2:F82,12)</f>
+        <f t="array" ref="V2:V104">_xll.TA_EMA(F2:F104,12)</f>
         <v>#N/A</v>
       </c>
       <c r="W2" t="e">
-        <f t="array" ref="W2:W82">_xll.TA_EMA(F2:F82,26)</f>
+        <f t="array" ref="W2:W104">_xll.TA_EMA(F2:F104,26)</f>
         <v>#N/A</v>
       </c>
       <c r="X2" t="e">
@@ -669,7 +668,7 @@
         <v>#N/A</v>
       </c>
       <c r="Y2" t="e">
-        <f t="array" ref="Y2:Y82">_xll.TA_EMA(X2:X82,9)</f>
+        <f t="array" ref="Y2:Y104">_xll.TA_EMA(X2:X104,9)</f>
         <v>#N/A</v>
       </c>
       <c r="Z2" t="e">
@@ -729,7 +728,6 @@
         <v>11281</v>
       </c>
       <c r="G3">
-        <f>_xll.TA_TYPPRICE(D3,E3,F3)</f>
         <v>11324.666666666666</v>
       </c>
       <c r="H3" t="e">
@@ -854,7 +852,6 @@
         <v>11525</v>
       </c>
       <c r="G4">
-        <f>_xll.TA_TYPPRICE(D4,E4,F4)</f>
         <v>11451.416666666666</v>
       </c>
       <c r="H4">
@@ -979,7 +976,6 @@
         <v>11340</v>
       </c>
       <c r="G5">
-        <f>_xll.TA_TYPPRICE(D5,E5,F5)</f>
         <v>11388.016666666668</v>
       </c>
       <c r="H5">
@@ -1104,7 +1100,6 @@
         <v>11539.15</v>
       </c>
       <c r="G6">
-        <f>_xll.TA_TYPPRICE(D6,E6,F6)</f>
         <v>11473.066666666666</v>
       </c>
       <c r="H6">
@@ -1229,7 +1224,6 @@
         <v>12000</v>
       </c>
       <c r="G7">
-        <f>_xll.TA_TYPPRICE(D7,E7,F7)</f>
         <v>11933.316666666666</v>
       </c>
       <c r="H7">
@@ -1354,7 +1348,6 @@
         <v>12222</v>
       </c>
       <c r="G8">
-        <f>_xll.TA_TYPPRICE(D8,E8,F8)</f>
         <v>12230.666666666666</v>
       </c>
       <c r="H8">
@@ -1479,7 +1472,6 @@
         <v>12500</v>
       </c>
       <c r="G9">
-        <f>_xll.TA_TYPPRICE(D9,E9,F9)</f>
         <v>12388.35</v>
       </c>
       <c r="H9">
@@ -1604,7 +1596,6 @@
         <v>12600</v>
       </c>
       <c r="G10">
-        <f>_xll.TA_TYPPRICE(D10,E10,F10)</f>
         <v>12577.35</v>
       </c>
       <c r="H10">
@@ -1729,7 +1720,6 @@
         <v>12820</v>
       </c>
       <c r="G11">
-        <f>_xll.TA_TYPPRICE(D11,E11,F11)</f>
         <v>12786.983333333332</v>
       </c>
       <c r="H11">
@@ -1854,7 +1844,6 @@
         <v>13840</v>
       </c>
       <c r="G12">
-        <f>_xll.TA_TYPPRICE(D12,E12,F12)</f>
         <v>13546</v>
       </c>
       <c r="H12">
@@ -1979,7 +1968,6 @@
         <v>14055</v>
       </c>
       <c r="G13">
-        <f>_xll.TA_TYPPRICE(D13,E13,F13)</f>
         <v>14015.333333333334</v>
       </c>
       <c r="H13">
@@ -2104,7 +2092,6 @@
         <v>13603</v>
       </c>
       <c r="G14">
-        <f>_xll.TA_TYPPRICE(D14,E14,F14)</f>
         <v>13751.6</v>
       </c>
       <c r="H14">
@@ -2229,7 +2216,6 @@
         <v>13440</v>
       </c>
       <c r="G15">
-        <f>_xll.TA_TYPPRICE(D15,E15,F15)</f>
         <v>13509.65</v>
       </c>
       <c r="H15">
@@ -2354,7 +2340,6 @@
         <v>13151</v>
       </c>
       <c r="G16">
-        <f>_xll.TA_TYPPRICE(D16,E16,F16)</f>
         <v>13250.666666666666</v>
       </c>
       <c r="H16">
@@ -2479,7 +2464,6 @@
         <v>13299</v>
       </c>
       <c r="G17">
-        <f>_xll.TA_TYPPRICE(D17,E17,F17)</f>
         <v>13200</v>
       </c>
       <c r="H17">
@@ -2604,7 +2588,6 @@
         <v>12801</v>
       </c>
       <c r="G18">
-        <f>_xll.TA_TYPPRICE(D18,E18,F18)</f>
         <v>12955.383333333333</v>
       </c>
       <c r="H18">
@@ -2729,7 +2712,6 @@
         <v>13050</v>
       </c>
       <c r="G19">
-        <f>_xll.TA_TYPPRICE(D19,E19,F19)</f>
         <v>13027.016666666668</v>
       </c>
       <c r="H19">
@@ -2854,7 +2836,6 @@
         <v>13982</v>
       </c>
       <c r="G20">
-        <f>_xll.TA_TYPPRICE(D20,E20,F20)</f>
         <v>13810.733333333332</v>
       </c>
       <c r="H20">
@@ -2979,7 +2960,6 @@
         <v>13805</v>
       </c>
       <c r="G21">
-        <f>_xll.TA_TYPPRICE(D21,E21,F21)</f>
         <v>13974.666666666666</v>
       </c>
       <c r="H21">
@@ -3104,7 +3084,6 @@
         <v>14095</v>
       </c>
       <c r="G22">
-        <f>_xll.TA_TYPPRICE(D22,E22,F22)</f>
         <v>14093.050000000001</v>
       </c>
       <c r="H22">
@@ -3229,7 +3208,6 @@
         <v>13716</v>
       </c>
       <c r="G23">
-        <f>_xll.TA_TYPPRICE(D23,E23,F23)</f>
         <v>13824.1</v>
       </c>
       <c r="H23">
@@ -3354,7 +3332,6 @@
         <v>13725</v>
       </c>
       <c r="G24">
-        <f>_xll.TA_TYPPRICE(D24,E24,F24)</f>
         <v>13801.416666666666</v>
       </c>
       <c r="H24">
@@ -3479,7 +3456,6 @@
         <v>13749</v>
       </c>
       <c r="G25">
-        <f>_xll.TA_TYPPRICE(D25,E25,F25)</f>
         <v>13797.666666666666</v>
       </c>
       <c r="H25">
@@ -3604,7 +3580,6 @@
         <v>13810</v>
       </c>
       <c r="G26">
-        <f>_xll.TA_TYPPRICE(D26,E26,F26)</f>
         <v>13813.316666666666</v>
       </c>
       <c r="H26">
@@ -3729,7 +3704,6 @@
         <v>13785</v>
       </c>
       <c r="G27">
-        <f>_xll.TA_TYPPRICE(D27,E27,F27)</f>
         <v>13802.066666666666</v>
       </c>
       <c r="H27">
@@ -3854,7 +3828,6 @@
         <v>13970</v>
       </c>
       <c r="G28">
-        <f>_xll.TA_TYPPRICE(D28,E28,F28)</f>
         <v>13920.699999999999</v>
       </c>
       <c r="H28">
@@ -3979,7 +3952,6 @@
         <v>14005</v>
       </c>
       <c r="G29">
-        <f>_xll.TA_TYPPRICE(D29,E29,F29)</f>
         <v>13985.75</v>
       </c>
       <c r="H29">
@@ -4104,7 +4076,6 @@
         <v>13851</v>
       </c>
       <c r="G30">
-        <f>_xll.TA_TYPPRICE(D30,E30,F30)</f>
         <v>13934.033333333333</v>
       </c>
       <c r="H30">
@@ -4229,7 +4200,6 @@
         <v>13860</v>
       </c>
       <c r="G31">
-        <f>_xll.TA_TYPPRICE(D31,E31,F31)</f>
         <v>13904.216666666667</v>
       </c>
       <c r="H31">
@@ -4354,7 +4324,6 @@
         <v>13940</v>
       </c>
       <c r="G32">
-        <f>_xll.TA_TYPPRICE(D32,E32,F32)</f>
         <v>14000.4</v>
       </c>
       <c r="H32">
@@ -4479,7 +4448,6 @@
         <v>13900</v>
       </c>
       <c r="G33">
-        <f>_xll.TA_TYPPRICE(D33,E33,F33)</f>
         <v>14266</v>
       </c>
       <c r="H33">
@@ -4604,7 +4572,6 @@
         <v>13970</v>
       </c>
       <c r="G34">
-        <f>_xll.TA_TYPPRICE(D34,E34,F34)</f>
         <v>13941.65</v>
       </c>
       <c r="H34">
@@ -4729,7 +4696,6 @@
         <v>13851</v>
       </c>
       <c r="G35">
-        <f>_xll.TA_TYPPRICE(D35,E35,F35)</f>
         <v>13891.050000000001</v>
       </c>
       <c r="H35">
@@ -4854,7 +4820,6 @@
         <v>13909</v>
       </c>
       <c r="G36">
-        <f>_xll.TA_TYPPRICE(D36,E36,F36)</f>
         <v>13918.266666666668</v>
       </c>
       <c r="H36">
@@ -4979,7 +4944,6 @@
         <v>13935</v>
       </c>
       <c r="G37">
-        <f>_xll.TA_TYPPRICE(D37,E37,F37)</f>
         <v>13943.016666666668</v>
       </c>
       <c r="H37">
@@ -5104,7 +5068,6 @@
         <v>13891</v>
       </c>
       <c r="G38">
-        <f>_xll.TA_TYPPRICE(D38,E38,F38)</f>
         <v>13906.949999999999</v>
       </c>
       <c r="H38">
@@ -5229,7 +5192,6 @@
         <v>13850</v>
       </c>
       <c r="G39">
-        <f>_xll.TA_TYPPRICE(D39,E39,F39)</f>
         <v>13884.333333333334</v>
       </c>
       <c r="H39">
@@ -5354,7 +5316,6 @@
         <v>13702</v>
       </c>
       <c r="G40">
-        <f>_xll.TA_TYPPRICE(D40,E40,F40)</f>
         <v>13767.683333333334</v>
       </c>
       <c r="H40">
@@ -5479,7 +5440,6 @@
         <v>13490</v>
       </c>
       <c r="G41">
-        <f>_xll.TA_TYPPRICE(D41,E41,F41)</f>
         <v>13564.666666666666</v>
       </c>
       <c r="H41">
@@ -5604,7 +5564,6 @@
         <v>13300</v>
       </c>
       <c r="G42">
-        <f>_xll.TA_TYPPRICE(D42,E42,F42)</f>
         <v>13229.85</v>
       </c>
       <c r="H42">
@@ -5729,7 +5688,6 @@
         <v>13492</v>
       </c>
       <c r="G43">
-        <f>_xll.TA_TYPPRICE(D43,E43,F43)</f>
         <v>13392.333333333334</v>
       </c>
       <c r="H43">
@@ -5854,7 +5812,6 @@
         <v>13250</v>
       </c>
       <c r="G44">
-        <f>_xll.TA_TYPPRICE(D44,E44,F44)</f>
         <v>13323.316666666666</v>
       </c>
       <c r="H44">
@@ -5979,7 +5936,6 @@
         <v>13500</v>
       </c>
       <c r="G45">
-        <f>_xll.TA_TYPPRICE(D45,E45,F45)</f>
         <v>13428</v>
       </c>
       <c r="H45">
@@ -6104,7 +6060,6 @@
         <v>13700</v>
       </c>
       <c r="G46">
-        <f>_xll.TA_TYPPRICE(D46,E46,F46)</f>
         <v>13663.333333333334</v>
       </c>
       <c r="H46">
@@ -6229,7 +6184,6 @@
         <v>13830</v>
       </c>
       <c r="G47">
-        <f>_xll.TA_TYPPRICE(D47,E47,F47)</f>
         <v>13825.683333333334</v>
       </c>
       <c r="H47">
@@ -6354,7 +6308,6 @@
         <v>13711</v>
       </c>
       <c r="G48">
-        <f>_xll.TA_TYPPRICE(D48,E48,F48)</f>
         <v>13783.666666666666</v>
       </c>
       <c r="H48">
@@ -6479,7 +6432,6 @@
         <v>13700</v>
       </c>
       <c r="G49">
-        <f>_xll.TA_TYPPRICE(D49,E49,F49)</f>
         <v>13763.266666666668</v>
       </c>
       <c r="H49">
@@ -6604,7 +6556,6 @@
         <v>13675</v>
       </c>
       <c r="G50">
-        <f>_xll.TA_TYPPRICE(D50,E50,F50)</f>
         <v>13696.199999999999</v>
       </c>
       <c r="H50">
@@ -6729,7 +6680,6 @@
         <v>13500</v>
       </c>
       <c r="G51">
-        <f>_xll.TA_TYPPRICE(D51,E51,F51)</f>
         <v>13555</v>
       </c>
       <c r="H51">
@@ -6854,7 +6804,6 @@
         <v>13790</v>
       </c>
       <c r="G52">
-        <f>_xll.TA_TYPPRICE(D52,E52,F52)</f>
         <v>13745.35</v>
       </c>
       <c r="H52">
@@ -6979,7 +6928,6 @@
         <v>13499</v>
       </c>
       <c r="G53">
-        <f>_xll.TA_TYPPRICE(D53,E53,F53)</f>
         <v>13616.550000000001</v>
       </c>
       <c r="H53">
@@ -7104,7 +7052,6 @@
         <v>13630</v>
       </c>
       <c r="G54">
-        <f>_xll.TA_TYPPRICE(D54,E54,F54)</f>
         <v>13641.5</v>
       </c>
       <c r="H54">
@@ -7229,7 +7176,6 @@
         <v>13705</v>
       </c>
       <c r="G55">
-        <f>_xll.TA_TYPPRICE(D55,E55,F55)</f>
         <v>13638.833333333334</v>
       </c>
       <c r="H55">
@@ -7354,7 +7300,6 @@
         <v>13550</v>
       </c>
       <c r="G56">
-        <f>_xll.TA_TYPPRICE(D56,E56,F56)</f>
         <v>13611.800000000001</v>
       </c>
       <c r="H56">
@@ -7479,7 +7424,6 @@
         <v>13400</v>
       </c>
       <c r="G57">
-        <f>_xll.TA_TYPPRICE(D57,E57,F57)</f>
         <v>13466.633333333333</v>
       </c>
       <c r="H57">
@@ -7600,7 +7544,6 @@
         <v>13360</v>
       </c>
       <c r="G58">
-        <f>_xll.TA_TYPPRICE(D58,E58,F58)</f>
         <v>13403.666666666666</v>
       </c>
       <c r="H58">
@@ -7721,7 +7664,6 @@
         <v>13333</v>
       </c>
       <c r="G59">
-        <f>_xll.TA_TYPPRICE(D59,E59,F59)</f>
         <v>13380.983333333332</v>
       </c>
       <c r="H59">
@@ -7842,7 +7784,6 @@
         <v>13325</v>
       </c>
       <c r="G60">
-        <f>_xll.TA_TYPPRICE(D60,E60,F60)</f>
         <v>13377.833333333334</v>
       </c>
       <c r="H60">
@@ -7963,7 +7904,6 @@
         <v>13275</v>
       </c>
       <c r="G61">
-        <f>_xll.TA_TYPPRICE(D61,E61,F61)</f>
         <v>13341.316666666666</v>
       </c>
       <c r="H61">
@@ -8084,7 +8024,6 @@
         <v>13357</v>
       </c>
       <c r="G62">
-        <f>_xll.TA_TYPPRICE(D62,E62,F62)</f>
         <v>13423.666666666666</v>
       </c>
       <c r="H62">
@@ -8205,7 +8144,6 @@
         <v>13300</v>
       </c>
       <c r="G63">
-        <f>_xll.TA_TYPPRICE(D63,E63,F63)</f>
         <v>13333.383333333333</v>
       </c>
       <c r="H63">
@@ -8326,7 +8264,6 @@
         <v>13350</v>
       </c>
       <c r="G64">
-        <f>_xll.TA_TYPPRICE(D64,E64,F64)</f>
         <v>13334.983333333332</v>
       </c>
       <c r="H64">
@@ -8447,7 +8384,6 @@
         <v>13390</v>
       </c>
       <c r="G65">
-        <f>_xll.TA_TYPPRICE(D65,E65,F65)</f>
         <v>13396.65</v>
       </c>
       <c r="H65">
@@ -8568,7 +8504,6 @@
         <v>13351.95</v>
       </c>
       <c r="G66">
-        <f>_xll.TA_TYPPRICE(D66,E66,F66)</f>
         <v>13284.316666666666</v>
       </c>
       <c r="H66">
@@ -8689,14 +8624,13 @@
         <v>13255</v>
       </c>
       <c r="G67">
-        <f>_xll.TA_TYPPRICE(D67,E67,F67)</f>
         <v>13362.65</v>
       </c>
       <c r="H67">
         <v>13345.774937479675</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I82" si="20">IF(F67&gt;H67,"UP","DOWN")</f>
+        <f t="shared" ref="I67:I104" si="20">IF(F67&gt;H67,"UP","DOWN")</f>
         <v>DOWN</v>
       </c>
       <c r="J67">
@@ -8706,42 +8640,42 @@
         <v>13256.669130599776</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" ref="L67:L82" si="21">IF(F67&gt;J67,"UP",IF(F67&lt;K67,"DOWN","No Confirmation"))</f>
+        <f t="shared" ref="L67:L104" si="21">IF(F67&gt;J67,"UP",IF(F67&lt;K67,"DOWN","No Confirmation"))</f>
         <v>DOWN</v>
       </c>
       <c r="M67" t="str">
-        <f t="shared" ref="M67:M82" si="22">IF(AND(I67="UP",L67="UP"),"UP",IF(AND(I67="DOWN",L67="DOWN"),"DOWN","No Trend"))</f>
+        <f t="shared" ref="M67:M104" si="22">IF(AND(I67="UP",L67="UP"),"UP",IF(AND(I67="DOWN",L67="DOWN"),"DOWN","No Trend"))</f>
         <v>DOWN</v>
       </c>
       <c r="N67">
         <v>31.888538464860794</v>
       </c>
       <c r="O67" t="str">
-        <f t="shared" ref="O67:O82" si="23">IF(N67&gt;60,"UP",IF(N67&lt;40,"DOWN","No Momentum"))</f>
+        <f t="shared" ref="O67:O104" si="23">IF(N67&gt;60,"UP",IF(N67&lt;40,"DOWN","No Momentum"))</f>
         <v>DOWN</v>
       </c>
       <c r="P67" t="str">
-        <f t="shared" ref="P67:P82" si="24">IF(AND(M67="UP",O67="UP"),"UP",IF(AND(M67="DOWN",O67="DOWN"),"DOWN","No Trend + Momentum"))</f>
+        <f t="shared" ref="P67:P104" si="24">IF(AND(M67="UP",O67="UP"),"UP",IF(AND(M67="DOWN",O67="DOWN"),"DOWN","No Trend + Momentum"))</f>
         <v>DOWN</v>
       </c>
       <c r="Q67">
-        <f t="shared" ref="Q67:Q82" si="25">F67-E67</f>
+        <f t="shared" ref="Q67:Q104" si="25">F67-E67</f>
         <v>7</v>
       </c>
       <c r="R67">
-        <f t="shared" ref="R67:R82" si="26">D67-E67</f>
+        <f t="shared" ref="R67:R104" si="26">D67-E67</f>
         <v>336.95000000000073</v>
       </c>
       <c r="S67">
-        <f t="shared" ref="S67:S82" si="27">Q67/R67</f>
+        <f t="shared" ref="S67:S104" si="27">Q67/R67</f>
         <v>2.0774595637334872E-2</v>
       </c>
       <c r="T67" t="str">
-        <f t="shared" ref="T67:T82" si="28">IF(S67&gt;0.8,"UP",IF(S67&lt;0.2,"DOWN","No Indication"))</f>
+        <f t="shared" ref="T67:T104" si="28">IF(S67&gt;0.8,"UP",IF(S67&lt;0.2,"DOWN","No Indication"))</f>
         <v>DOWN</v>
       </c>
       <c r="U67" t="str">
-        <f t="shared" ref="U67:U82" si="29">IF(AND(P67="UP",T67="UP"),"UP",IF(AND(P67="DOWN",T67="DOWN"),"DOWN","No T+M+I"))</f>
+        <f t="shared" ref="U67:U104" si="29">IF(AND(P67="UP",T67="UP"),"UP",IF(AND(P67="DOWN",T67="DOWN"),"DOWN","No T+M+I"))</f>
         <v>DOWN</v>
       </c>
       <c r="V67">
@@ -8751,42 +8685,42 @@
         <v>13441.44609092986</v>
       </c>
       <c r="X67">
-        <f t="shared" ref="X67:X82" si="30">V67-W67</f>
+        <f t="shared" ref="X67:X104" si="30">V67-W67</f>
         <v>-64.485752507507641</v>
       </c>
       <c r="Y67">
         <v>-40.512371778907365</v>
       </c>
       <c r="Z67" t="str">
-        <f t="shared" ref="Z67:Z82" si="31">IF(X67&gt;Y67,"UP",IF(X67&lt;Y67,"DOWN","No Indication"))</f>
+        <f t="shared" ref="Z67:Z104" si="31">IF(X67&gt;Y67,"UP",IF(X67&lt;Y67,"DOWN","No Indication"))</f>
         <v>DOWN</v>
       </c>
       <c r="AA67" t="str">
-        <f t="shared" ref="AA67:AA82" si="32">IF(AND(U67="UP",Z67="UP"),"UP",IF(AND(U67="DOWN",Z67="DOWN"),"DOWN","No TMIM"))</f>
+        <f t="shared" ref="AA67:AA104" si="32">IF(AND(U67="UP",Z67="UP"),"UP",IF(AND(U67="DOWN",Z67="DOWN"),"DOWN","No TMIM"))</f>
         <v>DOWN</v>
       </c>
       <c r="AB67" t="str">
-        <f t="shared" ref="AB67:AB82" si="33">IF(H67&gt;J67,"UP",IF(H67&lt;K67,"DOWN","No Confirmation"))</f>
+        <f t="shared" ref="AB67:AB104" si="33">IF(H67&gt;J67,"UP",IF(H67&lt;K67,"DOWN","No Confirmation"))</f>
         <v>No Confirmation</v>
       </c>
       <c r="AC67" t="str">
-        <f t="shared" ref="AC67:AC82" si="34">IF(AND(AA67="UP",AB67="UP"),"UP",IF(AND(AA67="DOWN",AB67="DOWN"),"DOWN","No Alert"))</f>
+        <f t="shared" ref="AC67:AC104" si="34">IF(AND(AA67="UP",AB67="UP"),"UP",IF(AND(AA67="DOWN",AB67="DOWN"),"DOWN","No Alert"))</f>
         <v>No Alert</v>
       </c>
       <c r="AD67" t="str">
-        <f t="shared" ref="AD67:AD82" si="35">IF(AC67="UP",MROUND(D67-((D67-E67)*0.886),0.05),IF(AC67="DOWN",MROUND(E67+((D67-E67)*0.886),0.05),"No Alert"))</f>
+        <f t="shared" ref="AD67:AD104" si="35">IF(AC67="UP",MROUND(D67-((D67-E67)*0.886),0.05),IF(AC67="DOWN",MROUND(E67+((D67-E67)*0.886),0.05),"No Alert"))</f>
         <v>No Alert</v>
       </c>
       <c r="AE67" t="str">
-        <f t="shared" ref="AE67:AE82" si="36">IF(AC67="UP",MROUND(D67-((D67-E67)*0.618),0.05),IF(AC67="DOWN",MROUND(E67+((D67-E67)*0.618),0.05),"No Alert"))</f>
+        <f t="shared" ref="AE67:AE104" si="36">IF(AC67="UP",MROUND(D67-((D67-E67)*0.618),0.05),IF(AC67="DOWN",MROUND(E67+((D67-E67)*0.618),0.05),"No Alert"))</f>
         <v>No Alert</v>
       </c>
       <c r="AF67" t="str">
-        <f t="shared" ref="AF67:AF82" si="37">IF(AC67="UP",MROUND(D67-((D67-E67)*0.5),0.05),IF(AC67="DOWN",MROUND(E67+((D67-E67)*0.5),0.05),"No Alert"))</f>
+        <f t="shared" ref="AF67:AF104" si="37">IF(AC67="UP",MROUND(D67-((D67-E67)*0.5),0.05),IF(AC67="DOWN",MROUND(E67+((D67-E67)*0.5),0.05),"No Alert"))</f>
         <v>No Alert</v>
       </c>
       <c r="AG67" t="str">
-        <f t="shared" ref="AG67:AG82" si="38">IF(AC67="UP",MROUND(D67-((D67-E67)*0.382),0.05),IF(AC67="DOWN",MROUND(E67+((D67-E67)*0.382),0.05),"No Alert"))</f>
+        <f t="shared" ref="AG67:AG104" si="38">IF(AC67="UP",MROUND(D67-((D67-E67)*0.382),0.05),IF(AC67="DOWN",MROUND(E67+((D67-E67)*0.382),0.05),"No Alert"))</f>
         <v>No Alert</v>
       </c>
     </row>
@@ -8810,7 +8744,6 @@
         <v>13330</v>
       </c>
       <c r="G68">
-        <f>_xll.TA_TYPPRICE(D68,E68,F68)</f>
         <v>13376.65</v>
       </c>
       <c r="H68">
@@ -8931,7 +8864,6 @@
         <v>13251</v>
       </c>
       <c r="G69">
-        <f>_xll.TA_TYPPRICE(D69,E69,F69)</f>
         <v>13290.716666666667</v>
       </c>
       <c r="H69">
@@ -9052,7 +8984,6 @@
         <v>13844.8</v>
       </c>
       <c r="G70">
-        <f>_xll.TA_TYPPRICE(D70,E70,F70)</f>
         <v>13727.6</v>
       </c>
       <c r="H70">
@@ -9173,7 +9104,6 @@
         <v>13605</v>
       </c>
       <c r="G71">
-        <f>_xll.TA_TYPPRICE(D71,E71,F71)</f>
         <v>13718.333333333334</v>
       </c>
       <c r="H71">
@@ -9294,7 +9224,6 @@
         <v>13350</v>
       </c>
       <c r="G72">
-        <f>_xll.TA_TYPPRICE(D72,E72,F72)</f>
         <v>13436.050000000001</v>
       </c>
       <c r="H72">
@@ -9415,7 +9344,6 @@
         <v>13070</v>
       </c>
       <c r="G73">
-        <f>_xll.TA_TYPPRICE(D73,E73,F73)</f>
         <v>13206.233333333332</v>
       </c>
       <c r="H73">
@@ -9536,7 +9464,6 @@
         <v>13640</v>
       </c>
       <c r="G74">
-        <f>_xll.TA_TYPPRICE(D74,E74,F74)</f>
         <v>13430.666666666666</v>
       </c>
       <c r="H74">
@@ -9657,7 +9584,6 @@
         <v>13803.05</v>
       </c>
       <c r="G75">
-        <f>_xll.TA_TYPPRICE(D75,E75,F75)</f>
         <v>13834.366666666667</v>
       </c>
       <c r="H75">
@@ -9778,7 +9704,6 @@
         <v>13899.9</v>
       </c>
       <c r="G76">
-        <f>_xll.TA_TYPPRICE(D76,E76,F76)</f>
         <v>13925.9</v>
       </c>
       <c r="H76">
@@ -9899,7 +9824,6 @@
         <v>13750</v>
       </c>
       <c r="G77">
-        <f>_xll.TA_TYPPRICE(D77,E77,F77)</f>
         <v>13816.666666666666</v>
       </c>
       <c r="H77">
@@ -10020,7 +9944,6 @@
         <v>13848</v>
       </c>
       <c r="G78">
-        <f>_xll.TA_TYPPRICE(D78,E78,F78)</f>
         <v>13799.699999999999</v>
       </c>
       <c r="H78">
@@ -10141,7 +10064,6 @@
         <v>13850</v>
       </c>
       <c r="G79">
-        <f>_xll.TA_TYPPRICE(D79,E79,F79)</f>
         <v>13840.133333333333</v>
       </c>
       <c r="H79">
@@ -10262,7 +10184,6 @@
         <v>13860</v>
       </c>
       <c r="G80">
-        <f>_xll.TA_TYPPRICE(D80,E80,F80)</f>
         <v>13852.333333333334</v>
       </c>
       <c r="H80">
@@ -10383,7 +10304,6 @@
         <v>14250</v>
       </c>
       <c r="G81">
-        <f>_xll.TA_TYPPRICE(D81,E81,F81)</f>
         <v>14156.15</v>
       </c>
       <c r="H81">
@@ -10504,7 +10424,6 @@
         <v>14780</v>
       </c>
       <c r="G82">
-        <f>_xll.TA_TYPPRICE(D82,E82,F82)</f>
         <v>14685</v>
       </c>
       <c r="H82">
@@ -10606,141 +10525,3135 @@
       </c>
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B83" s="1"/>
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="1">
+        <v>42975</v>
+      </c>
+      <c r="C83">
+        <v>14725</v>
+      </c>
+      <c r="D83">
+        <v>14885.1</v>
+      </c>
+      <c r="E83">
+        <v>14724.7</v>
+      </c>
+      <c r="F83">
+        <v>14725</v>
+      </c>
+      <c r="G83">
+        <v>14778.266666666668</v>
+      </c>
+      <c r="H83">
+        <v>14559.328745395978</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J83">
+        <v>14355.70996468798</v>
+      </c>
+      <c r="K83">
+        <v>14016.883186209465</v>
+      </c>
+      <c r="L83" t="str">
+        <f t="shared" si="21"/>
+        <v>UP</v>
+      </c>
+      <c r="M83" t="str">
+        <f t="shared" si="22"/>
+        <v>UP</v>
+      </c>
+      <c r="N83">
+        <v>83.506313210996723</v>
+      </c>
+      <c r="O83" t="str">
+        <f t="shared" si="23"/>
+        <v>UP</v>
+      </c>
+      <c r="P83" t="str">
+        <f t="shared" si="24"/>
+        <v>UP</v>
+      </c>
+      <c r="Q83">
+        <f t="shared" si="25"/>
+        <v>0.2999999999992724</v>
+      </c>
+      <c r="R83">
+        <f t="shared" si="26"/>
+        <v>160.39999999999964</v>
+      </c>
+      <c r="S83">
+        <f t="shared" si="27"/>
+        <v>1.8703241895216527E-3</v>
+      </c>
+      <c r="T83" t="str">
+        <f t="shared" si="28"/>
+        <v>DOWN</v>
+      </c>
+      <c r="U83" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V83">
+        <v>14050.120643682447</v>
+      </c>
+      <c r="W83">
+        <v>13795.821526624157</v>
+      </c>
+      <c r="X83">
+        <f t="shared" si="30"/>
+        <v>254.29911705828999</v>
+      </c>
+      <c r="Y83">
+        <v>124.26208306600935</v>
+      </c>
+      <c r="Z83" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA83" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB83" t="str">
+        <f t="shared" si="33"/>
+        <v>UP</v>
+      </c>
+      <c r="AC83" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD83" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE83" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF83" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG83" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B84" s="1"/>
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="1">
+        <v>42976</v>
+      </c>
+      <c r="C84">
+        <v>14765</v>
+      </c>
+      <c r="D84">
+        <v>14765</v>
+      </c>
+      <c r="E84">
+        <v>14405</v>
+      </c>
+      <c r="F84">
+        <v>14628</v>
+      </c>
+      <c r="G84">
+        <v>14599.333333333334</v>
+      </c>
+      <c r="H84">
+        <v>14579.331039364657</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J84">
+        <v>14446.663305868429</v>
+      </c>
+      <c r="K84">
+        <v>14103.131367051807</v>
+      </c>
+      <c r="L84" t="str">
+        <f t="shared" si="21"/>
+        <v>UP</v>
+      </c>
+      <c r="M84" t="str">
+        <f t="shared" si="22"/>
+        <v>UP</v>
+      </c>
+      <c r="N84">
+        <v>74.837659952387028</v>
+      </c>
+      <c r="O84" t="str">
+        <f t="shared" si="23"/>
+        <v>UP</v>
+      </c>
+      <c r="P84" t="str">
+        <f t="shared" si="24"/>
+        <v>UP</v>
+      </c>
+      <c r="Q84">
+        <f t="shared" si="25"/>
+        <v>223</v>
+      </c>
+      <c r="R84">
+        <f t="shared" si="26"/>
+        <v>360</v>
+      </c>
+      <c r="S84">
+        <f t="shared" si="27"/>
+        <v>0.61944444444444446</v>
+      </c>
+      <c r="T84" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U84" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V84">
+        <v>14139.025160038993</v>
+      </c>
+      <c r="W84">
+        <v>13857.464376503849</v>
+      </c>
+      <c r="X84">
+        <f t="shared" si="30"/>
+        <v>281.56078353514386</v>
+      </c>
+      <c r="Y84">
+        <v>155.72182315983625</v>
+      </c>
+      <c r="Z84" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA84" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB84" t="str">
+        <f t="shared" si="33"/>
+        <v>UP</v>
+      </c>
+      <c r="AC84" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD84" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE84" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF84" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG84" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B85" s="1"/>
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="1">
+        <v>42977</v>
+      </c>
+      <c r="C85">
+        <v>14628.05</v>
+      </c>
+      <c r="D85">
+        <v>14796.05</v>
+      </c>
+      <c r="E85">
+        <v>14425</v>
+      </c>
+      <c r="F85">
+        <v>14750</v>
+      </c>
+      <c r="G85">
+        <v>14657.016666666668</v>
+      </c>
+      <c r="H85">
+        <v>14618.173853015662</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J85">
+        <v>14524.304793453222</v>
+      </c>
+      <c r="K85">
+        <v>14174.657729929182</v>
+      </c>
+      <c r="L85" t="str">
+        <f t="shared" si="21"/>
+        <v>UP</v>
+      </c>
+      <c r="M85" t="str">
+        <f t="shared" si="22"/>
+        <v>UP</v>
+      </c>
+      <c r="N85">
+        <v>78.368073840506227</v>
+      </c>
+      <c r="O85" t="str">
+        <f t="shared" si="23"/>
+        <v>UP</v>
+      </c>
+      <c r="P85" t="str">
+        <f t="shared" si="24"/>
+        <v>UP</v>
+      </c>
+      <c r="Q85">
+        <f t="shared" si="25"/>
+        <v>325</v>
+      </c>
+      <c r="R85">
+        <f t="shared" si="26"/>
+        <v>371.04999999999927</v>
+      </c>
+      <c r="S85">
+        <f t="shared" si="27"/>
+        <v>0.87589273682792246</v>
+      </c>
+      <c r="T85" t="str">
+        <f t="shared" si="28"/>
+        <v>UP</v>
+      </c>
+      <c r="U85" t="str">
+        <f t="shared" si="29"/>
+        <v>UP</v>
+      </c>
+      <c r="V85">
+        <v>14233.021289263763</v>
+      </c>
+      <c r="W85">
+        <v>13923.578126392453</v>
+      </c>
+      <c r="X85">
+        <f t="shared" si="30"/>
+        <v>309.44316287131005</v>
+      </c>
+      <c r="Y85">
+        <v>186.466091102131</v>
+      </c>
+      <c r="Z85" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA85" t="str">
+        <f t="shared" si="32"/>
+        <v>UP</v>
+      </c>
+      <c r="AB85" t="str">
+        <f t="shared" si="33"/>
+        <v>UP</v>
+      </c>
+      <c r="AC85" t="str">
+        <f t="shared" si="34"/>
+        <v>UP</v>
+      </c>
+      <c r="AD85">
+        <f t="shared" si="35"/>
+        <v>14467.300000000001</v>
+      </c>
+      <c r="AE85">
+        <f t="shared" si="36"/>
+        <v>14566.75</v>
+      </c>
+      <c r="AF85">
+        <f t="shared" si="37"/>
+        <v>14610.550000000001</v>
+      </c>
+      <c r="AG85">
+        <f t="shared" si="38"/>
+        <v>14654.300000000001</v>
+      </c>
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B86" s="1"/>
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="1">
+        <v>42978</v>
+      </c>
+      <c r="C86">
+        <v>14797.95</v>
+      </c>
+      <c r="D86">
+        <v>14797.95</v>
+      </c>
+      <c r="E86">
+        <v>14620.15</v>
+      </c>
+      <c r="F86">
+        <v>14725</v>
+      </c>
+      <c r="G86">
+        <v>14714.366666666667</v>
+      </c>
+      <c r="H86">
+        <v>14666.270259841163</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J86">
+        <v>14585.114839352507</v>
+      </c>
+      <c r="K86">
+        <v>14273.656012167141</v>
+      </c>
+      <c r="L86" t="str">
+        <f t="shared" si="21"/>
+        <v>UP</v>
+      </c>
+      <c r="M86" t="str">
+        <f t="shared" si="22"/>
+        <v>UP</v>
+      </c>
+      <c r="N86">
+        <v>75.649320438052101</v>
+      </c>
+      <c r="O86" t="str">
+        <f t="shared" si="23"/>
+        <v>UP</v>
+      </c>
+      <c r="P86" t="str">
+        <f t="shared" si="24"/>
+        <v>UP</v>
+      </c>
+      <c r="Q86">
+        <f t="shared" si="25"/>
+        <v>104.85000000000036</v>
+      </c>
+      <c r="R86">
+        <f t="shared" si="26"/>
+        <v>177.80000000000109</v>
+      </c>
+      <c r="S86">
+        <f t="shared" si="27"/>
+        <v>0.58970753655792874</v>
+      </c>
+      <c r="T86" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U86" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V86">
+        <v>14308.710321684723</v>
+      </c>
+      <c r="W86">
+        <v>13982.942709622641</v>
+      </c>
+      <c r="X86">
+        <f t="shared" si="30"/>
+        <v>325.76761206208175</v>
+      </c>
+      <c r="Y86">
+        <v>214.32639529412114</v>
+      </c>
+      <c r="Z86" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA86" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB86" t="str">
+        <f t="shared" si="33"/>
+        <v>UP</v>
+      </c>
+      <c r="AC86" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD86" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE86" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF86" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG86" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B87" s="1"/>
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="1">
+        <v>42979</v>
+      </c>
+      <c r="C87">
+        <v>14780</v>
+      </c>
+      <c r="D87">
+        <v>14780</v>
+      </c>
+      <c r="E87">
+        <v>14640</v>
+      </c>
+      <c r="F87">
+        <v>14700</v>
+      </c>
+      <c r="G87">
+        <v>14706.666666666666</v>
+      </c>
+      <c r="H87">
+        <v>14686.468463253914</v>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J87">
+        <v>14628.422652829728</v>
+      </c>
+      <c r="K87">
+        <v>14355.06578724111</v>
+      </c>
+      <c r="L87" t="str">
+        <f t="shared" si="21"/>
+        <v>UP</v>
+      </c>
+      <c r="M87" t="str">
+        <f t="shared" si="22"/>
+        <v>UP</v>
+      </c>
+      <c r="N87">
+        <v>72.505126175870842</v>
+      </c>
+      <c r="O87" t="str">
+        <f t="shared" si="23"/>
+        <v>UP</v>
+      </c>
+      <c r="P87" t="str">
+        <f t="shared" si="24"/>
+        <v>UP</v>
+      </c>
+      <c r="Q87">
+        <f t="shared" si="25"/>
+        <v>60</v>
+      </c>
+      <c r="R87">
+        <f t="shared" si="26"/>
+        <v>140</v>
+      </c>
+      <c r="S87">
+        <f t="shared" si="27"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="T87" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U87" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V87">
+        <v>14368.908733733228</v>
+      </c>
+      <c r="W87">
+        <v>14036.058064465407</v>
+      </c>
+      <c r="X87">
+        <f t="shared" si="30"/>
+        <v>332.85066926782019</v>
+      </c>
+      <c r="Y87">
+        <v>238.03125008886096</v>
+      </c>
+      <c r="Z87" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA87" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB87" t="str">
+        <f t="shared" si="33"/>
+        <v>UP</v>
+      </c>
+      <c r="AC87" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD87" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE87" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF87" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG87" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B88" s="1"/>
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="1">
+        <v>42982</v>
+      </c>
+      <c r="C88">
+        <v>14779.95</v>
+      </c>
+      <c r="D88">
+        <v>14780</v>
+      </c>
+      <c r="E88">
+        <v>14500.05</v>
+      </c>
+      <c r="F88">
+        <v>14650</v>
+      </c>
+      <c r="G88">
+        <v>14643.35</v>
+      </c>
+      <c r="H88">
+        <v>14664.909231626956</v>
+      </c>
+      <c r="I88" t="str">
+        <f t="shared" si="20"/>
+        <v>DOWN</v>
+      </c>
+      <c r="J88">
+        <v>14662.106507756454</v>
+      </c>
+      <c r="K88">
+        <v>14387.284501187531</v>
+      </c>
+      <c r="L88" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M88" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N88">
+        <v>65.680472510478367</v>
+      </c>
+      <c r="O88" t="str">
+        <f t="shared" si="23"/>
+        <v>UP</v>
+      </c>
+      <c r="P88" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q88">
+        <f t="shared" si="25"/>
+        <v>149.95000000000073</v>
+      </c>
+      <c r="R88">
+        <f t="shared" si="26"/>
+        <v>279.95000000000073</v>
+      </c>
+      <c r="S88">
+        <f t="shared" si="27"/>
+        <v>0.53563136274334822</v>
+      </c>
+      <c r="T88" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U88" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V88">
+        <v>14412.153543928116</v>
+      </c>
+      <c r="W88">
+        <v>14081.535244875377</v>
+      </c>
+      <c r="X88">
+        <f t="shared" si="30"/>
+        <v>330.61829905273953</v>
+      </c>
+      <c r="Y88">
+        <v>256.54865988163669</v>
+      </c>
+      <c r="Z88" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA88" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB88" t="str">
+        <f t="shared" si="33"/>
+        <v>UP</v>
+      </c>
+      <c r="AC88" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD88" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE88" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF88" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG88" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B89" s="1"/>
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" s="1">
+        <v>42983</v>
+      </c>
+      <c r="C89">
+        <v>14779.05</v>
+      </c>
+      <c r="D89">
+        <v>14779.05</v>
+      </c>
+      <c r="E89">
+        <v>14480</v>
+      </c>
+      <c r="F89">
+        <v>14500.05</v>
+      </c>
+      <c r="G89">
+        <v>14586.366666666667</v>
+      </c>
+      <c r="H89">
+        <v>14625.637949146811</v>
+      </c>
+      <c r="I89" t="str">
+        <f t="shared" si="20"/>
+        <v>DOWN</v>
+      </c>
+      <c r="J89">
+        <v>14688.093950477241</v>
+      </c>
+      <c r="K89">
+        <v>14407.88794536808</v>
+      </c>
+      <c r="L89" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M89" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N89">
+        <v>48.549467158021287</v>
+      </c>
+      <c r="O89" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P89" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q89">
+        <f t="shared" si="25"/>
+        <v>20.049999999999272</v>
+      </c>
+      <c r="R89">
+        <f t="shared" si="26"/>
+        <v>299.04999999999927</v>
+      </c>
+      <c r="S89">
+        <f t="shared" si="27"/>
+        <v>6.7045644541044377E-2</v>
+      </c>
+      <c r="T89" t="str">
+        <f t="shared" si="28"/>
+        <v>DOWN</v>
+      </c>
+      <c r="U89" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V89">
+        <v>14425.676075631483</v>
+      </c>
+      <c r="W89">
+        <v>14112.53633784757</v>
+      </c>
+      <c r="X89">
+        <f t="shared" si="30"/>
+        <v>313.13973778391301</v>
+      </c>
+      <c r="Y89">
+        <v>267.86687546209197</v>
+      </c>
+      <c r="Z89" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA89" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB89" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC89" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD89" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE89" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF89" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG89" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B90" s="1"/>
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" s="1">
+        <v>42984</v>
+      </c>
+      <c r="C90">
+        <v>14415</v>
+      </c>
+      <c r="D90">
+        <v>14700</v>
+      </c>
+      <c r="E90">
+        <v>14415</v>
+      </c>
+      <c r="F90">
+        <v>14500</v>
+      </c>
+      <c r="G90">
+        <v>14538.333333333334</v>
+      </c>
+      <c r="H90">
+        <v>14581.985641240073</v>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="20"/>
+        <v>DOWN</v>
+      </c>
+      <c r="J90">
+        <v>14690.739739260076</v>
+      </c>
+      <c r="K90">
+        <v>14409.46840195295</v>
+      </c>
+      <c r="L90" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M90" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N90">
+        <v>48.544189789933171</v>
+      </c>
+      <c r="O90" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P90" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q90">
+        <f t="shared" si="25"/>
+        <v>85</v>
+      </c>
+      <c r="R90">
+        <f t="shared" si="26"/>
+        <v>285</v>
+      </c>
+      <c r="S90">
+        <f t="shared" si="27"/>
+        <v>0.2982456140350877</v>
+      </c>
+      <c r="T90" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U90" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V90">
+        <v>14437.110525534332</v>
+      </c>
+      <c r="W90">
+        <v>14141.237349858862</v>
+      </c>
+      <c r="X90">
+        <f t="shared" si="30"/>
+        <v>295.87317567546961</v>
+      </c>
+      <c r="Y90">
+        <v>273.46813550476747</v>
+      </c>
+      <c r="Z90" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA90" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB90" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC90" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD90" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE90" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF90" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG90" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="91" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B91" s="1"/>
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" s="1">
+        <v>42985</v>
+      </c>
+      <c r="C91">
+        <v>14699.85</v>
+      </c>
+      <c r="D91">
+        <v>14749.95</v>
+      </c>
+      <c r="E91">
+        <v>14480.45</v>
+      </c>
+      <c r="F91">
+        <v>14655</v>
+      </c>
+      <c r="G91">
+        <v>14628.466666666667</v>
+      </c>
+      <c r="H91">
+        <v>14605.22615395337</v>
+      </c>
+      <c r="I91" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J91">
+        <v>14703.897574980059</v>
+      </c>
+      <c r="K91">
+        <v>14425.24209040785</v>
+      </c>
+      <c r="L91" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M91" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N91">
+        <v>63.794512286869455</v>
+      </c>
+      <c r="O91" t="str">
+        <f t="shared" si="23"/>
+        <v>UP</v>
+      </c>
+      <c r="P91" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q91">
+        <f t="shared" si="25"/>
+        <v>174.54999999999927</v>
+      </c>
+      <c r="R91">
+        <f t="shared" si="26"/>
+        <v>269.5</v>
+      </c>
+      <c r="S91">
+        <f t="shared" si="27"/>
+        <v>0.64768089053803068</v>
+      </c>
+      <c r="T91" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U91" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V91">
+        <v>14470.631983144434</v>
+      </c>
+      <c r="W91">
+        <v>14179.29384246191</v>
+      </c>
+      <c r="X91">
+        <f t="shared" si="30"/>
+        <v>291.33814068252468</v>
+      </c>
+      <c r="Y91">
+        <v>277.04213654031889</v>
+      </c>
+      <c r="Z91" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA91" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB91" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC91" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD91" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE91" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF91" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG91" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="92" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B92" s="1"/>
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" s="1">
+        <v>42986</v>
+      </c>
+      <c r="C92">
+        <v>14664.95</v>
+      </c>
+      <c r="D92">
+        <v>14665</v>
+      </c>
+      <c r="E92">
+        <v>14504.3</v>
+      </c>
+      <c r="F92">
+        <v>14599</v>
+      </c>
+      <c r="G92">
+        <v>14589.433333333334</v>
+      </c>
+      <c r="H92">
+        <v>14597.329743643353</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J92">
+        <v>14695.253669428936</v>
+      </c>
+      <c r="K92">
+        <v>14442.810514761661</v>
+      </c>
+      <c r="L92" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M92" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N92">
+        <v>56.263739533906474</v>
+      </c>
+      <c r="O92" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P92" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q92">
+        <f t="shared" si="25"/>
+        <v>94.700000000000728</v>
+      </c>
+      <c r="R92">
+        <f t="shared" si="26"/>
+        <v>160.70000000000073</v>
+      </c>
+      <c r="S92">
+        <f t="shared" si="27"/>
+        <v>0.58929682638456937</v>
+      </c>
+      <c r="T92" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U92" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V92">
+        <v>14490.380908814521</v>
+      </c>
+      <c r="W92">
+        <v>14210.383187464731</v>
+      </c>
+      <c r="X92">
+        <f t="shared" si="30"/>
+        <v>279.99772134978957</v>
+      </c>
+      <c r="Y92">
+        <v>277.63325350221305</v>
+      </c>
+      <c r="Z92" t="str">
+        <f t="shared" si="31"/>
+        <v>UP</v>
+      </c>
+      <c r="AA92" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB92" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC92" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD92" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE92" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF92" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG92" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="93" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B93" s="1"/>
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" s="1">
+        <v>42989</v>
+      </c>
+      <c r="C93">
+        <v>14520.05</v>
+      </c>
+      <c r="D93">
+        <v>14689.95</v>
+      </c>
+      <c r="E93">
+        <v>14520.05</v>
+      </c>
+      <c r="F93">
+        <v>14650</v>
+      </c>
+      <c r="G93">
+        <v>14620</v>
+      </c>
+      <c r="H93">
+        <v>14608.664871821677</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J93">
+        <v>14694.075076222505</v>
+      </c>
+      <c r="K93">
+        <v>14459.974844814626</v>
+      </c>
+      <c r="L93" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M93" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N93">
+        <v>61.444933380070054</v>
+      </c>
+      <c r="O93" t="str">
+        <f t="shared" si="23"/>
+        <v>UP</v>
+      </c>
+      <c r="P93" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q93">
+        <f t="shared" si="25"/>
+        <v>129.95000000000073</v>
+      </c>
+      <c r="R93">
+        <f t="shared" si="26"/>
+        <v>169.90000000000146</v>
+      </c>
+      <c r="S93">
+        <f t="shared" si="27"/>
+        <v>0.76486168334314075</v>
+      </c>
+      <c r="T93" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U93" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V93">
+        <v>14514.937692073825</v>
+      </c>
+      <c r="W93">
+        <v>14242.947395800677</v>
+      </c>
+      <c r="X93">
+        <f t="shared" si="30"/>
+        <v>271.99029627314849</v>
+      </c>
+      <c r="Y93">
+        <v>276.50466205640015</v>
+      </c>
+      <c r="Z93" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA93" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB93" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC93" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD93" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE93" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF93" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG93" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="94" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B94" s="1"/>
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="1">
+        <v>42990</v>
+      </c>
+      <c r="C94">
+        <v>14600.05</v>
+      </c>
+      <c r="D94">
+        <v>14699</v>
+      </c>
+      <c r="E94">
+        <v>14404.5</v>
+      </c>
+      <c r="F94">
+        <v>14500</v>
+      </c>
+      <c r="G94">
+        <v>14534.5</v>
+      </c>
+      <c r="H94">
+        <v>14571.582435910837</v>
+      </c>
+      <c r="I94" t="str">
+        <f t="shared" si="20"/>
+        <v>DOWN</v>
+      </c>
+      <c r="J94">
+        <v>14695.169503728615</v>
+      </c>
+      <c r="K94">
+        <v>14447.647101522487</v>
+      </c>
+      <c r="L94" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M94" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N94">
+        <v>42.802923833159987</v>
+      </c>
+      <c r="O94" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P94" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q94">
+        <f t="shared" si="25"/>
+        <v>95.5</v>
+      </c>
+      <c r="R94">
+        <f t="shared" si="26"/>
+        <v>294.5</v>
+      </c>
+      <c r="S94">
+        <f t="shared" si="27"/>
+        <v>0.32427843803056028</v>
+      </c>
+      <c r="T94" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U94" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V94">
+        <v>14512.639585600929</v>
+      </c>
+      <c r="W94">
+        <v>14261.98832944507</v>
+      </c>
+      <c r="X94">
+        <f t="shared" si="30"/>
+        <v>250.6512561558593</v>
+      </c>
+      <c r="Y94">
+        <v>271.333980876292</v>
+      </c>
+      <c r="Z94" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA94" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB94" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC94" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD94" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE94" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF94" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG94" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="95" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B95" s="1"/>
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" s="1">
+        <v>42991</v>
+      </c>
+      <c r="C95">
+        <v>14500.05</v>
+      </c>
+      <c r="D95">
+        <v>14750</v>
+      </c>
+      <c r="E95">
+        <v>14450</v>
+      </c>
+      <c r="F95">
+        <v>14636</v>
+      </c>
+      <c r="G95">
+        <v>14612</v>
+      </c>
+      <c r="H95">
+        <v>14591.791217955419</v>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J95">
+        <v>14707.35405845559</v>
+      </c>
+      <c r="K95">
+        <v>14448.169967850823</v>
+      </c>
+      <c r="L95" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M95" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N95">
+        <v>57.437783119555718</v>
+      </c>
+      <c r="O95" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P95" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q95">
+        <f t="shared" si="25"/>
+        <v>186</v>
+      </c>
+      <c r="R95">
+        <f t="shared" si="26"/>
+        <v>300</v>
+      </c>
+      <c r="S95">
+        <f t="shared" si="27"/>
+        <v>0.62</v>
+      </c>
+      <c r="T95" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U95" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V95">
+        <v>14531.618110893094</v>
+      </c>
+      <c r="W95">
+        <v>14289.692897634324</v>
+      </c>
+      <c r="X95">
+        <f t="shared" si="30"/>
+        <v>241.92521325876987</v>
+      </c>
+      <c r="Y95">
+        <v>265.45222735278759</v>
+      </c>
+      <c r="Z95" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA95" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB95" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC95" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD95" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE95" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF95" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG95" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
     </row>
     <row r="96" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="1"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="1"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="1"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="1"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="1"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="1"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="1"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="1"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="1"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="1"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="1"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="1"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="1"/>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="1"/>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="1"/>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="1"/>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" s="1">
+        <v>42992</v>
+      </c>
+      <c r="C96">
+        <v>14575</v>
+      </c>
+      <c r="D96">
+        <v>14749.95</v>
+      </c>
+      <c r="E96">
+        <v>14550</v>
+      </c>
+      <c r="F96">
+        <v>14588.05</v>
+      </c>
+      <c r="G96">
+        <v>14629.333333333334</v>
+      </c>
+      <c r="H96">
+        <v>14610.562275644377</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" si="20"/>
+        <v>DOWN</v>
+      </c>
+      <c r="J96">
+        <v>14716.819823243237</v>
+      </c>
+      <c r="K96">
+        <v>14470.798863883974</v>
+      </c>
+      <c r="L96" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M96" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N96">
+        <v>51.617171271599247</v>
+      </c>
+      <c r="O96" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P96" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q96">
+        <f t="shared" si="25"/>
+        <v>38.049999999999272</v>
+      </c>
+      <c r="R96">
+        <f t="shared" si="26"/>
+        <v>199.95000000000073</v>
+      </c>
+      <c r="S96">
+        <f t="shared" si="27"/>
+        <v>0.19029757439359407</v>
+      </c>
+      <c r="T96" t="str">
+        <f t="shared" si="28"/>
+        <v>DOWN</v>
+      </c>
+      <c r="U96" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V96">
+        <v>14540.299939986464</v>
+      </c>
+      <c r="W96">
+        <v>14311.793423735486</v>
+      </c>
+      <c r="X96">
+        <f t="shared" si="30"/>
+        <v>228.50651625097817</v>
+      </c>
+      <c r="Y96">
+        <v>258.06308513242573</v>
+      </c>
+      <c r="Z96" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA96" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB96" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC96" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD96" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE96" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF96" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG96" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
+    </row>
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" s="1">
+        <v>42993</v>
+      </c>
+      <c r="C97">
+        <v>14590</v>
+      </c>
+      <c r="D97">
+        <v>14750</v>
+      </c>
+      <c r="E97">
+        <v>14492.35</v>
+      </c>
+      <c r="F97">
+        <v>14723</v>
+      </c>
+      <c r="G97">
+        <v>14655.116666666667</v>
+      </c>
+      <c r="H97">
+        <v>14632.839471155523</v>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J97">
+        <v>14724.193195855851</v>
+      </c>
+      <c r="K97">
+        <v>14475.588005243091</v>
+      </c>
+      <c r="L97" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M97" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N97">
+        <v>64.332723120310604</v>
+      </c>
+      <c r="O97" t="str">
+        <f t="shared" si="23"/>
+        <v>UP</v>
+      </c>
+      <c r="P97" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q97">
+        <f t="shared" si="25"/>
+        <v>230.64999999999964</v>
+      </c>
+      <c r="R97">
+        <f t="shared" si="26"/>
+        <v>257.64999999999964</v>
+      </c>
+      <c r="S97">
+        <f t="shared" si="27"/>
+        <v>0.89520667572287971</v>
+      </c>
+      <c r="T97" t="str">
+        <f t="shared" si="28"/>
+        <v>UP</v>
+      </c>
+      <c r="U97" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V97">
+        <v>14568.407641527008</v>
+      </c>
+      <c r="W97">
+        <v>14342.25317012545</v>
+      </c>
+      <c r="X97">
+        <f t="shared" si="30"/>
+        <v>226.15447140155811</v>
+      </c>
+      <c r="Y97">
+        <v>251.6813623862522</v>
+      </c>
+      <c r="Z97" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA97" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB97" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC97" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD97" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE97" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF97" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG97" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
+    </row>
+    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" s="1">
+        <v>42996</v>
+      </c>
+      <c r="C98">
+        <v>14685</v>
+      </c>
+      <c r="D98">
+        <v>14780</v>
+      </c>
+      <c r="E98">
+        <v>14123.05</v>
+      </c>
+      <c r="F98">
+        <v>14649</v>
+      </c>
+      <c r="G98">
+        <v>14517.35</v>
+      </c>
+      <c r="H98">
+        <v>14575.094735577761</v>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J98">
+        <v>14736.594707887883</v>
+      </c>
+      <c r="K98">
+        <v>14397.246226300182</v>
+      </c>
+      <c r="L98" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M98" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N98">
+        <v>54.512738632788235</v>
+      </c>
+      <c r="O98" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P98" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q98">
+        <f t="shared" si="25"/>
+        <v>525.95000000000073</v>
+      </c>
+      <c r="R98">
+        <f t="shared" si="26"/>
+        <v>656.95000000000073</v>
+      </c>
+      <c r="S98">
+        <f t="shared" si="27"/>
+        <v>0.80059365248496861</v>
+      </c>
+      <c r="T98" t="str">
+        <f t="shared" si="28"/>
+        <v>UP</v>
+      </c>
+      <c r="U98" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V98">
+        <v>14580.806465907468</v>
+      </c>
+      <c r="W98">
+        <v>14364.975157523564</v>
+      </c>
+      <c r="X98">
+        <f t="shared" si="30"/>
+        <v>215.83130838390389</v>
+      </c>
+      <c r="Y98">
+        <v>244.51135158578253</v>
+      </c>
+      <c r="Z98" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA98" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB98" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC98" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD98" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE98" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF98" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG98" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
+    </row>
+    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" s="1">
+        <v>42997</v>
+      </c>
+      <c r="C99">
+        <v>14600</v>
+      </c>
+      <c r="D99">
+        <v>14700</v>
+      </c>
+      <c r="E99">
+        <v>14600</v>
+      </c>
+      <c r="F99">
+        <v>14650</v>
+      </c>
+      <c r="G99">
+        <v>14650</v>
+      </c>
+      <c r="H99">
+        <v>14612.54736778888</v>
+      </c>
+      <c r="I99" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J99">
+        <v>14728.462550579465</v>
+      </c>
+      <c r="K99">
+        <v>14442.302620455697</v>
+      </c>
+      <c r="L99" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M99" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N99">
+        <v>54.629723204368673</v>
+      </c>
+      <c r="O99" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P99" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q99">
+        <f t="shared" si="25"/>
+        <v>50</v>
+      </c>
+      <c r="R99">
+        <f t="shared" si="26"/>
+        <v>100</v>
+      </c>
+      <c r="S99">
+        <f t="shared" si="27"/>
+        <v>0.5</v>
+      </c>
+      <c r="T99" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U99" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V99">
+        <v>14591.451624998626</v>
+      </c>
+      <c r="W99">
+        <v>14386.088108818114</v>
+      </c>
+      <c r="X99">
+        <f t="shared" si="30"/>
+        <v>205.36351618051231</v>
+      </c>
+      <c r="Y99">
+        <v>236.68178450472848</v>
+      </c>
+      <c r="Z99" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA99" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB99" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC99" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD99" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE99" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF99" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG99" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
+    </row>
+    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" s="1">
+        <v>42998</v>
+      </c>
+      <c r="C100">
+        <v>14739.95</v>
+      </c>
+      <c r="D100">
+        <v>14739.95</v>
+      </c>
+      <c r="E100">
+        <v>14600</v>
+      </c>
+      <c r="F100">
+        <v>14600.25</v>
+      </c>
+      <c r="G100">
+        <v>14646.733333333332</v>
+      </c>
+      <c r="H100">
+        <v>14629.640350561105</v>
+      </c>
+      <c r="I100" t="str">
+        <f t="shared" si="20"/>
+        <v>DOWN</v>
+      </c>
+      <c r="J100">
+        <v>14731.015317117362</v>
+      </c>
+      <c r="K100">
+        <v>14477.346482576653</v>
+      </c>
+      <c r="L100" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M100" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N100">
+        <v>47.097252229838759</v>
+      </c>
+      <c r="O100" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P100" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q100">
+        <f t="shared" si="25"/>
+        <v>0.25</v>
+      </c>
+      <c r="R100">
+        <f t="shared" si="26"/>
+        <v>139.95000000000073</v>
+      </c>
+      <c r="S100">
+        <f t="shared" si="27"/>
+        <v>1.7863522686673719E-3</v>
+      </c>
+      <c r="T100" t="str">
+        <f t="shared" si="28"/>
+        <v>DOWN</v>
+      </c>
+      <c r="U100" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V100">
+        <v>14592.805221152685</v>
+      </c>
+      <c r="W100">
+        <v>14401.951952609365</v>
+      </c>
+      <c r="X100">
+        <f t="shared" si="30"/>
+        <v>190.85326854332016</v>
+      </c>
+      <c r="Y100">
+        <v>227.51608131244683</v>
+      </c>
+      <c r="Z100" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA100" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB100" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC100" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD100" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE100" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF100" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG100" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
+    </row>
+    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" s="1">
+        <v>42999</v>
+      </c>
+      <c r="C101">
+        <v>14749.95</v>
+      </c>
+      <c r="D101">
+        <v>14750</v>
+      </c>
+      <c r="E101">
+        <v>14325.05</v>
+      </c>
+      <c r="F101">
+        <v>14600</v>
+      </c>
+      <c r="G101">
+        <v>14558.35</v>
+      </c>
+      <c r="H101">
+        <v>14593.995175280554</v>
+      </c>
+      <c r="I101" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J101">
+        <v>14735.234135535726</v>
+      </c>
+      <c r="K101">
+        <v>14443.502819781841</v>
+      </c>
+      <c r="L101" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M101" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N101">
+        <v>47.056496845217168</v>
+      </c>
+      <c r="O101" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P101" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q101">
+        <f t="shared" si="25"/>
+        <v>274.95000000000073</v>
+      </c>
+      <c r="R101">
+        <f t="shared" si="26"/>
+        <v>424.95000000000073</v>
+      </c>
+      <c r="S101">
+        <f t="shared" si="27"/>
+        <v>0.64701729615248915</v>
+      </c>
+      <c r="T101" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U101" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V101">
+        <v>14593.912110206118</v>
+      </c>
+      <c r="W101">
+        <v>14416.622178342004</v>
+      </c>
+      <c r="X101">
+        <f t="shared" si="30"/>
+        <v>177.2899318641139</v>
+      </c>
+      <c r="Y101">
+        <v>217.47085142278024</v>
+      </c>
+      <c r="Z101" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA101" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB101" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC101" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD101" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE101" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF101" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG101" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
+    </row>
+    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="1">
+        <v>43000</v>
+      </c>
+      <c r="C102">
+        <v>14550.05</v>
+      </c>
+      <c r="D102">
+        <v>14596.9</v>
+      </c>
+      <c r="E102">
+        <v>14420</v>
+      </c>
+      <c r="F102">
+        <v>14460</v>
+      </c>
+      <c r="G102">
+        <v>14492.300000000001</v>
+      </c>
+      <c r="H102">
+        <v>14543.147587640276</v>
+      </c>
+      <c r="I102" t="str">
+        <f t="shared" si="20"/>
+        <v>DOWN</v>
+      </c>
+      <c r="J102">
+        <v>14704.493216527786</v>
+      </c>
+      <c r="K102">
+        <v>14438.279970941432</v>
+      </c>
+      <c r="L102" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M102" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N102">
+        <v>29.305147329465797</v>
+      </c>
+      <c r="O102" t="str">
+        <f t="shared" si="23"/>
+        <v>DOWN</v>
+      </c>
+      <c r="P102" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q102">
+        <f t="shared" si="25"/>
+        <v>40</v>
+      </c>
+      <c r="R102">
+        <f t="shared" si="26"/>
+        <v>176.89999999999964</v>
+      </c>
+      <c r="S102">
+        <f t="shared" si="27"/>
+        <v>0.22611644997173591</v>
+      </c>
+      <c r="T102" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U102" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V102">
+        <v>14573.310247097485</v>
+      </c>
+      <c r="W102">
+        <v>14419.835350316671</v>
+      </c>
+      <c r="X102">
+        <f t="shared" si="30"/>
+        <v>153.47489678081365</v>
+      </c>
+      <c r="Y102">
+        <v>204.67166049438691</v>
+      </c>
+      <c r="Z102" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA102" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB102" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC102" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD102" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE102" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF102" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG102" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
+    </row>
+    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" s="1">
+        <v>43003</v>
+      </c>
+      <c r="C103">
+        <v>14400.05</v>
+      </c>
+      <c r="D103">
+        <v>14649.9</v>
+      </c>
+      <c r="E103">
+        <v>14000</v>
+      </c>
+      <c r="F103">
+        <v>14600</v>
+      </c>
+      <c r="G103">
+        <v>14416.633333333333</v>
+      </c>
+      <c r="H103">
+        <v>14479.890460486804</v>
+      </c>
+      <c r="I103" t="str">
+        <f t="shared" si="20"/>
+        <v>UP</v>
+      </c>
+      <c r="J103">
+        <v>14692.361390632723</v>
+      </c>
+      <c r="K103">
+        <v>14340.884421843337</v>
+      </c>
+      <c r="L103" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M103" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N103">
+        <v>51.958708009017307</v>
+      </c>
+      <c r="O103" t="str">
+        <f t="shared" si="23"/>
+        <v>No Momentum</v>
+      </c>
+      <c r="P103" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q103">
+        <f t="shared" si="25"/>
+        <v>600</v>
+      </c>
+      <c r="R103">
+        <f t="shared" si="26"/>
+        <v>649.89999999999964</v>
+      </c>
+      <c r="S103">
+        <f t="shared" si="27"/>
+        <v>0.92321895676257937</v>
+      </c>
+      <c r="T103" t="str">
+        <f t="shared" si="28"/>
+        <v>UP</v>
+      </c>
+      <c r="U103" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V103">
+        <v>14577.416362928641</v>
+      </c>
+      <c r="W103">
+        <v>14433.180879922844</v>
+      </c>
+      <c r="X103">
+        <f t="shared" si="30"/>
+        <v>144.23548300579751</v>
+      </c>
+      <c r="Y103">
+        <v>192.58442499666904</v>
+      </c>
+      <c r="Z103" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA103" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB103" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC103" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD103" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE103" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF103" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG103" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
+    </row>
+    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="1">
+        <v>43004</v>
+      </c>
+      <c r="C104">
+        <v>14400.05</v>
+      </c>
+      <c r="D104">
+        <v>14499.95</v>
+      </c>
+      <c r="E104">
+        <v>14300.1</v>
+      </c>
+      <c r="F104">
+        <v>14399.95</v>
+      </c>
+      <c r="G104">
+        <v>14400</v>
+      </c>
+      <c r="H104">
+        <v>14439.945230243402</v>
+      </c>
+      <c r="I104" t="str">
+        <f t="shared" si="20"/>
+        <v>DOWN</v>
+      </c>
+      <c r="J104">
+        <v>14649.603303825452</v>
+      </c>
+      <c r="K104">
+        <v>14331.821216989261</v>
+      </c>
+      <c r="L104" t="str">
+        <f t="shared" si="21"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="M104" t="str">
+        <f t="shared" si="22"/>
+        <v>No Trend</v>
+      </c>
+      <c r="N104">
+        <v>33.045047378942712</v>
+      </c>
+      <c r="O104" t="str">
+        <f t="shared" si="23"/>
+        <v>DOWN</v>
+      </c>
+      <c r="P104" t="str">
+        <f t="shared" si="24"/>
+        <v>No Trend + Momentum</v>
+      </c>
+      <c r="Q104">
+        <f t="shared" si="25"/>
+        <v>99.850000000000364</v>
+      </c>
+      <c r="R104">
+        <f t="shared" si="26"/>
+        <v>199.85000000000036</v>
+      </c>
+      <c r="S104">
+        <f t="shared" si="27"/>
+        <v>0.49962471853890511</v>
+      </c>
+      <c r="T104" t="str">
+        <f t="shared" si="28"/>
+        <v>No Indication</v>
+      </c>
+      <c r="U104" t="str">
+        <f t="shared" si="29"/>
+        <v>No T+M+I</v>
+      </c>
+      <c r="V104">
+        <v>14550.113845555004</v>
+      </c>
+      <c r="W104">
+        <v>14430.719333261892</v>
+      </c>
+      <c r="X104">
+        <f t="shared" si="30"/>
+        <v>119.39451229311271</v>
+      </c>
+      <c r="Y104">
+        <v>177.94644245595777</v>
+      </c>
+      <c r="Z104" t="str">
+        <f t="shared" si="31"/>
+        <v>DOWN</v>
+      </c>
+      <c r="AA104" t="str">
+        <f t="shared" si="32"/>
+        <v>No TMIM</v>
+      </c>
+      <c r="AB104" t="str">
+        <f t="shared" si="33"/>
+        <v>No Confirmation</v>
+      </c>
+      <c r="AC104" t="str">
+        <f t="shared" si="34"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AD104" t="str">
+        <f t="shared" si="35"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AE104" t="str">
+        <f t="shared" si="36"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AF104" t="str">
+        <f t="shared" si="37"/>
+        <v>No Alert</v>
+      </c>
+      <c r="AG104" t="str">
+        <f t="shared" si="38"/>
+        <v>No Alert</v>
+      </c>
+    </row>
+    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" s="1">
+        <v>43005</v>
+      </c>
+      <c r="C105">
+        <v>14740</v>
+      </c>
+      <c r="D105">
+        <v>14740</v>
+      </c>
+      <c r="E105">
+        <v>14110</v>
+      </c>
+      <c r="F105">
+        <v>14498</v>
+      </c>
+      <c r="G105">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" s="1">
+        <v>43006</v>
+      </c>
+      <c r="C106">
+        <v>14401.05</v>
+      </c>
+      <c r="D106">
+        <v>14499</v>
+      </c>
+      <c r="E106">
+        <v>14365</v>
+      </c>
+      <c r="F106">
+        <v>14484.9</v>
+      </c>
+      <c r="G106">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" s="1">
+        <v>43007</v>
+      </c>
+      <c r="C107">
+        <v>14611</v>
+      </c>
+      <c r="D107">
+        <v>14611</v>
+      </c>
+      <c r="E107">
+        <v>14238.05</v>
+      </c>
+      <c r="F107">
+        <v>14400.05</v>
+      </c>
+      <c r="G107">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" s="1">
+        <v>43011</v>
+      </c>
+      <c r="C108">
+        <v>14699</v>
+      </c>
+      <c r="D108">
+        <v>14699</v>
+      </c>
+      <c r="E108">
+        <v>14300</v>
+      </c>
+      <c r="F108">
+        <v>14315.05</v>
+      </c>
+      <c r="G108">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" s="1">
+        <v>43012</v>
+      </c>
+      <c r="C109">
+        <v>14300.15</v>
+      </c>
+      <c r="D109">
+        <v>14512.95</v>
+      </c>
+      <c r="E109">
+        <v>14289.7</v>
+      </c>
+      <c r="F109">
+        <v>14350</v>
+      </c>
+      <c r="G109">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" s="1">
+        <v>43013</v>
+      </c>
+      <c r="C110">
+        <v>14499.95</v>
+      </c>
+      <c r="D110">
+        <v>14499.95</v>
+      </c>
+      <c r="E110">
+        <v>14300</v>
+      </c>
+      <c r="F110">
+        <v>14499</v>
+      </c>
+      <c r="G110">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>5</v>
+      </c>
+      <c r="B111" s="1">
+        <v>43014</v>
+      </c>
+      <c r="C111">
+        <v>14498.95</v>
+      </c>
+      <c r="D111">
+        <v>14499</v>
+      </c>
+      <c r="E111">
+        <v>14399.4</v>
+      </c>
+      <c r="F111">
+        <v>14485</v>
+      </c>
+      <c r="G111">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" s="1">
+        <v>43017</v>
+      </c>
+      <c r="C112">
+        <v>14739.1</v>
+      </c>
+      <c r="D112">
+        <v>14739.1</v>
+      </c>
+      <c r="E112">
+        <v>14380</v>
+      </c>
+      <c r="F112">
+        <v>14400</v>
+      </c>
+      <c r="G112">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" s="1">
+        <v>43018</v>
+      </c>
+      <c r="C113">
+        <v>14480</v>
+      </c>
+      <c r="D113">
+        <v>14690</v>
+      </c>
+      <c r="E113">
+        <v>14376</v>
+      </c>
+      <c r="F113">
+        <v>14382.3</v>
+      </c>
+      <c r="G113">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114" s="1">
+        <v>43019</v>
+      </c>
+      <c r="C114">
+        <v>14524.9</v>
+      </c>
+      <c r="D114">
+        <v>14524.9</v>
+      </c>
+      <c r="E114">
+        <v>14225</v>
+      </c>
+      <c r="F114">
+        <v>14225</v>
+      </c>
+      <c r="G114">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" s="1">
+        <v>43020</v>
+      </c>
+      <c r="C115">
+        <v>14391.95</v>
+      </c>
+      <c r="D115">
+        <v>14400</v>
+      </c>
+      <c r="E115">
+        <v>14250.05</v>
+      </c>
+      <c r="F115">
+        <v>14400</v>
+      </c>
+      <c r="G115">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" s="1">
+        <v>43021</v>
+      </c>
+      <c r="C116">
+        <v>14399.95</v>
+      </c>
+      <c r="D116">
+        <v>14400</v>
+      </c>
+      <c r="E116">
+        <v>14220</v>
+      </c>
+      <c r="F116">
+        <v>14250.25</v>
+      </c>
+      <c r="G116">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" s="1">
+        <v>43024</v>
+      </c>
+      <c r="C117">
+        <v>14320</v>
+      </c>
+      <c r="D117">
+        <v>14320</v>
+      </c>
+      <c r="E117">
+        <v>14185.2</v>
+      </c>
+      <c r="F117">
+        <v>14200</v>
+      </c>
+      <c r="G117">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" s="1">
+        <v>43025</v>
+      </c>
+      <c r="C118">
+        <v>14200.05</v>
+      </c>
+      <c r="D118">
+        <v>14200.05</v>
+      </c>
+      <c r="E118">
+        <v>14000.1</v>
+      </c>
+      <c r="F118">
+        <v>14100</v>
+      </c>
+      <c r="G118">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119" s="1">
+        <v>43026</v>
+      </c>
+      <c r="C119">
+        <v>14053.65</v>
+      </c>
+      <c r="D119">
+        <v>14300</v>
+      </c>
+      <c r="E119">
+        <v>14015</v>
+      </c>
+      <c r="F119">
+        <v>14100</v>
+      </c>
+      <c r="G119">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" s="1">
+        <v>43027</v>
+      </c>
+      <c r="C120">
+        <v>14200</v>
+      </c>
+      <c r="D120">
+        <v>14434.7</v>
+      </c>
+      <c r="E120">
+        <v>14163.1</v>
+      </c>
+      <c r="F120">
+        <v>14387</v>
+      </c>
+      <c r="G120">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" s="1">
+        <v>43031</v>
+      </c>
+      <c r="C121">
+        <v>14497.95</v>
+      </c>
+      <c r="D121">
+        <v>14497.95</v>
+      </c>
+      <c r="E121">
+        <v>14269.1</v>
+      </c>
+      <c r="F121">
+        <v>14349</v>
+      </c>
+      <c r="G121">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>5</v>
+      </c>
+      <c r="B122" s="1">
+        <v>43032</v>
+      </c>
+      <c r="C122">
+        <v>14337.05</v>
+      </c>
+      <c r="D122">
+        <v>14350</v>
+      </c>
+      <c r="E122">
+        <v>14205</v>
+      </c>
+      <c r="F122">
+        <v>14270.05</v>
+      </c>
+      <c r="G122">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>5</v>
+      </c>
+      <c r="B123" s="1">
+        <v>43033</v>
+      </c>
+      <c r="C123">
+        <v>14255</v>
+      </c>
+      <c r="D123">
+        <v>14444</v>
+      </c>
+      <c r="E123">
+        <v>14100</v>
+      </c>
+      <c r="F123">
+        <v>14237.2</v>
+      </c>
+      <c r="G123">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" s="1">
+        <v>43034</v>
+      </c>
+      <c r="C124">
+        <v>14232.95</v>
+      </c>
+      <c r="D124">
+        <v>14428</v>
+      </c>
+      <c r="E124">
+        <v>14001.15</v>
+      </c>
+      <c r="F124">
+        <v>14350</v>
+      </c>
+      <c r="G124">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125" s="1">
+        <v>43035</v>
+      </c>
+      <c r="C125">
+        <v>14333.3</v>
+      </c>
+      <c r="D125">
+        <v>14524.2</v>
+      </c>
+      <c r="E125">
+        <v>14300</v>
+      </c>
+      <c r="F125">
+        <v>14300</v>
+      </c>
+      <c r="G125">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>